<commit_message>
terminado ajustes de diferido
</commit_message>
<xml_diff>
--- a/src/assets/templates/Plantilla Carga Masiva.xlsx
+++ b/src/assets/templates/Plantilla Carga Masiva.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
   <si>
     <t>TIPO_CLIENTE</t>
   </si>
@@ -233,33 +233,6 @@
   </si>
   <si>
     <t>CIUDAD</t>
-  </si>
-  <si>
-    <t>Caracas</t>
-  </si>
-  <si>
-    <t>Chacao</t>
-  </si>
-  <si>
-    <t>V269933506</t>
-  </si>
-  <si>
-    <t>RICHARD RAFAEL MATTEY RODRIGUEZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calle el rincon barrio jose feliz rivas zona 9 </t>
-  </si>
-  <si>
-    <t>01770001441102052363</t>
-  </si>
-  <si>
-    <t>5D275690</t>
-  </si>
-  <si>
-    <t>5D275690F</t>
-  </si>
-  <si>
-    <t>richardmat99@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -608,7 +581,7 @@
   <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,69 +680,11 @@
       </c>
     </row>
     <row r="2" spans="1:23" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G2" s="4">
-        <v>1070</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q2" s="4">
-        <v>82361634</v>
-      </c>
-      <c r="R2" s="4">
-        <v>1</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="T2" s="4">
-        <v>200</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="V2" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="W2" s="4" t="s">
-        <v>69</v>
-      </c>
+      <c r="A2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="U2" s="6"/>
     </row>
     <row r="3" spans="1:23" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:23" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -851,11 +766,8 @@
       <c r="P21" s="5"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="U2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">

</xml_diff>

<commit_message>
avances en carga masiva
</commit_message>
<xml_diff>
--- a/src/assets/templates/Plantilla Carga Masiva.xlsx
+++ b/src/assets/templates/Plantilla Carga Masiva.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="88">
   <si>
     <t>TIPO_CLIENTE</t>
   </si>
@@ -239,6 +239,57 @@
   </si>
   <si>
     <t>NUMERO_TELEFONO_2</t>
+  </si>
+  <si>
+    <t>REP_DOC_ID</t>
+  </si>
+  <si>
+    <t>REP_PRIMER_NOMBRE</t>
+  </si>
+  <si>
+    <t>REP_SEGUNDO_NOMBRE</t>
+  </si>
+  <si>
+    <t>REP_PRIMER_APELLIDO</t>
+  </si>
+  <si>
+    <t>REP_SEGUNDO_APELLIDO</t>
+  </si>
+  <si>
+    <t>REP_EMAIL</t>
+  </si>
+  <si>
+    <t>REP_RIF</t>
+  </si>
+  <si>
+    <t>CNAT_DOC_ID</t>
+  </si>
+  <si>
+    <t>CNAT_PRIMER_NOMBRE</t>
+  </si>
+  <si>
+    <t>CNAT_SEGUNDO_NOMBRE</t>
+  </si>
+  <si>
+    <t>CNAT_PRIMER_APELLIDO</t>
+  </si>
+  <si>
+    <t>CNAT_SEGUNDO_APELLIDO</t>
+  </si>
+  <si>
+    <t>CNAT_FECHA_NACIMIENTO</t>
+  </si>
+  <si>
+    <t>CNAT_TIPO_NATURAL</t>
+  </si>
+  <si>
+    <t>CNAT_GENERO</t>
+  </si>
+  <si>
+    <t>CNAT_PROFESION</t>
+  </si>
+  <si>
+    <t>CNAT_T_DOC</t>
   </si>
 </sst>
 </file>
@@ -584,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y21"/>
+  <dimension ref="A1:AP21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="X5" sqref="X5"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="AQ3" sqref="AQ3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,10 +663,27 @@
     <col min="19" max="19" width="11.5703125" customWidth="1"/>
     <col min="21" max="21" width="36.140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>65</v>
       </c>
@@ -691,64 +759,115 @@
       <c r="Y1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:42" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="I2" s="5"/>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
       <c r="U2" s="6"/>
     </row>
-    <row r="3" spans="1:25" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:25" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:25" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:25" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:25" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" s="4" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:42" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:42" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:42" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:42" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I7" s="5"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
     </row>
-    <row r="8" spans="1:25" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
     </row>
-    <row r="9" spans="1:25" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:42" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
     </row>
-    <row r="10" spans="1:25" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:42" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
     </row>
-    <row r="11" spans="1:25" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:42" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
     </row>
-    <row r="12" spans="1:25" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:42" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I12" s="5"/>
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
     </row>
-    <row r="13" spans="1:25" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:42" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I13" s="5"/>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
     </row>
-    <row r="14" spans="1:25" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:42" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I14" s="5"/>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
     </row>
-    <row r="15" spans="1:25" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:42" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I15" s="5"/>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
     </row>
-    <row r="16" spans="1:25" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:42" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>

</xml_diff>